<commit_message>
notebook and latest data
</commit_message>
<xml_diff>
--- a/answersxl.xlsx
+++ b/answersxl.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4514" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4513" uniqueCount="567">
   <si>
     <t xml:space="preserve">Отметка времени</t>
   </si>
@@ -1840,16 +1840,16 @@
   </sheetPr>
   <dimension ref="A1:MG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="FK1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="FK1" activeCellId="0" sqref="FK1"/>
-      <selection pane="bottomLeft" activeCell="FN18" activeCellId="0" sqref="FN18"/>
+      <selection pane="topLeft" activeCell="CM1" activeCellId="0" sqref="CM1"/>
+      <selection pane="bottomLeft" activeCell="CO11" activeCellId="0" sqref="CO11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="119" min="1" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="120" min="120" style="0" width="39.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="120" min="120" style="0" width="39.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="351" min="121" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="352" style="0" width="14.43"/>
   </cols>
@@ -3700,9 +3700,7 @@
       <c r="AU4" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="CS4" s="2" t="s">
-        <v>172</v>
-      </c>
+      <c r="CS4" s="2"/>
       <c r="CZ4" s="2" t="s">
         <v>191</v>
       </c>

</xml_diff>